<commit_message>
subtle update in data
</commit_message>
<xml_diff>
--- a/data/from_readers/ReviewedByALLuza/Descriptors_crosstaxa_review_ALLUZA_ALLUZA.xlsx
+++ b/data/from_readers/ReviewedByALLuza/Descriptors_crosstaxa_review_ALLUZA_ALLUZA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topoa\Dropbox\ReefSyn\wg_syn\data\from_readers\ReviewedByALLuza\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Microsoft\Dropbox\ReefSyn\wg_syn\data\from_readers\ReviewedByALLuza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E177DF02-99DE-4F34-B800-6A85A9FC2DDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC281AF8-7EC0-441C-8E1A-024F0FB89150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20835" yWindow="105" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfPapers" sheetId="1" r:id="rId1"/>
@@ -1210,11 +1210,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1432,7 +1432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2947,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="U35" workbookViewId="0">
+      <selection activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2991,7 +2993,7 @@
       <c r="D1" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="41" t="s">
         <v>288</v>
       </c>
       <c r="F1" s="16" t="s">
@@ -6784,7 +6786,7 @@
         <v>93</v>
       </c>
       <c r="X46" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y46" s="19" t="s">
         <v>121</v>
@@ -6867,7 +6869,7 @@
         <v>93</v>
       </c>
       <c r="X47" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y47" s="19" t="s">
         <v>121</v>
@@ -6950,7 +6952,7 @@
         <v>93</v>
       </c>
       <c r="X48" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y48" s="19" t="s">
         <v>121</v>
@@ -7033,7 +7035,7 @@
         <v>93</v>
       </c>
       <c r="X49" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y49" s="19" t="s">
         <v>121</v>
@@ -7116,7 +7118,7 @@
         <v>93</v>
       </c>
       <c r="X50" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y50" s="19" t="s">
         <v>121</v>
@@ -7199,7 +7201,7 @@
         <v>93</v>
       </c>
       <c r="X51" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y51" s="19" t="s">
         <v>121</v>
@@ -7282,7 +7284,7 @@
         <v>93</v>
       </c>
       <c r="X52" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y52" s="19" t="s">
         <v>121</v>
@@ -7365,7 +7367,7 @@
         <v>93</v>
       </c>
       <c r="X53" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y53" s="19" t="s">
         <v>121</v>
@@ -7448,7 +7450,7 @@
         <v>93</v>
       </c>
       <c r="X54" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y54" s="19" t="s">
         <v>121</v>
@@ -7531,7 +7533,7 @@
         <v>93</v>
       </c>
       <c r="X55" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y55" s="19" t="s">
         <v>121</v>
@@ -7614,7 +7616,7 @@
         <v>93</v>
       </c>
       <c r="X56" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y56" s="19" t="s">
         <v>121</v>
@@ -7697,7 +7699,7 @@
         <v>93</v>
       </c>
       <c r="X57" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y57" s="19" t="s">
         <v>121</v>
@@ -7780,7 +7782,7 @@
         <v>93</v>
       </c>
       <c r="X58" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y58" s="19" t="s">
         <v>121</v>
@@ -7863,7 +7865,7 @@
         <v>93</v>
       </c>
       <c r="X59" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y59" s="19" t="s">
         <v>121</v>
@@ -7946,7 +7948,7 @@
         <v>93</v>
       </c>
       <c r="X60" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y60" s="19" t="s">
         <v>121</v>
@@ -8029,7 +8031,7 @@
         <v>93</v>
       </c>
       <c r="X61" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y61" s="19" t="s">
         <v>121</v>
@@ -8112,7 +8114,7 @@
         <v>93</v>
       </c>
       <c r="X62" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y62" s="19" t="s">
         <v>121</v>
@@ -8195,7 +8197,7 @@
         <v>93</v>
       </c>
       <c r="X63" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y63" s="19" t="s">
         <v>121</v>
@@ -8278,7 +8280,7 @@
         <v>93</v>
       </c>
       <c r="X64" s="19" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Y64" s="19" t="s">
         <v>121</v>
@@ -38518,11 +38520,11 @@
       <c r="AA1" s="34"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
@@ -38643,7 +38645,7 @@
       <c r="A10" s="40" t="s">
         <v>260</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>288</v>
       </c>
       <c r="C10" s="40" t="s">

</xml_diff>